<commit_message>
Support for multiline headers
</commit_message>
<xml_diff>
--- a/src/test/resources/Book1.xlsx
+++ b/src/test/resources/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguel/raw-labs/das-excel/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966E3548-7A07-B442-9638-0F179F6E7D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774DEF72-D6D8-FB41-92D7-83EDEB8CC997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17220" xr2:uid="{0500A7D5-CF3F-614D-9139-4008F734EA5A}"/>
+    <workbookView xWindow="680" yWindow="760" windowWidth="28040" windowHeight="17220" activeTab="1" xr2:uid="{0500A7D5-CF3F-614D-9139-4008F734EA5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Multi Line" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -103,6 +104,21 @@
   </si>
   <si>
     <t>Cucu</t>
+  </si>
+  <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third Part</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -479,7 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAC99C1-02A9-514B-9C96-7BFAE101A1F0}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -605,6 +621,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F47C4B8B-87F6-BB43-8100-3E46861AB99D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAE5D99-C2FD-2743-9B7A-CFE77ACFB680}">
   <dimension ref="B4:C6"/>
   <sheetViews>

</xml_diff>